<commit_message>
Add documentation for procedure di subentro
</commit_message>
<xml_diff>
--- a/docs/_static/xlsx/tab_Tipo_di_certificato.xlsx
+++ b/docs/_static/xlsx/tab_Tipo_di_certificato.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>di Stato Libero</t>
+  </si>
+  <si>
+    <t>Anagrafico di Unione Civile</t>
+  </si>
+  <si>
+    <t>di Contratto di Convivenza</t>
   </si>
 </sst>
 </file>
@@ -427,11 +433,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -596,6 +602,22 @@
         <v>21</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>